<commit_message>
Make usade date and count field names consistant
</commit_message>
<xml_diff>
--- a/tests/bin/OpenRefine_exports/1_BR1_2019.xlsx
+++ b/tests/bin/OpenRefine_exports/1_BR1_2019.xlsx
@@ -48,12 +48,6 @@
     <t>Data_Type</t>
   </si>
   <si>
-    <t>R4_Month</t>
-  </si>
-  <si>
-    <t>R4_Count</t>
-  </si>
-  <si>
     <t>Illumina Biological Content - unstructured</t>
   </si>
   <si>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>Section_Type</t>
+  </si>
+  <si>
+    <t>Usage_Date</t>
+  </si>
+  <si>
+    <t>Usage_Count</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J10"/>
+      <selection activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,45 +440,45 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
         <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1">
         <v>43313</v>
@@ -489,34 +489,34 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K3" s="1">
         <v>43344</v>
@@ -527,34 +527,34 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="1">
         <v>43374</v>
@@ -565,34 +565,34 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K5" s="1">
         <v>43405</v>
@@ -603,34 +603,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K6" s="1">
         <v>43435</v>
@@ -641,34 +641,34 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K7" s="1">
         <v>43466</v>
@@ -679,34 +679,34 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K8" s="1">
         <v>43497</v>
@@ -717,34 +717,34 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K9" s="1">
         <v>43525</v>
@@ -755,34 +755,34 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K10" s="1">
         <v>43525</v>

</xml_diff>